<commit_message>
[improve] Modify file constructer and functionality 	1.Reconstruct the code constructor 	2.Add DirectX11 renderer, add a test a function to render a 	image 	3.There's a issue that render loop seems needed to improve
</commit_message>
<xml_diff>
--- a/documents/CSJVideoParser_dev_points.xlsx
+++ b/documents/CSJVideoParser_dev_points.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="16455"/>
+    <workbookView windowWidth="17610" windowHeight="14895"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>CSJVideoParser Version1.0.0</t>
   </si>
@@ -148,13 +148,22 @@
     <t>视频渲染</t>
   </si>
   <si>
-    <t>使用DirectX渲染，目前已经集成，支持纯色背景渲染，需要添加视频帧的渲染功能</t>
+    <t>windows端使用DirectX渲染，目前已经集成，支持纯色背景渲染，需要添加视频帧的渲染功能</t>
+  </si>
+  <si>
+    <t>已完成</t>
+  </si>
+  <si>
+    <t>macOS端使用Metal渲染，目前已经集成，支持纯色渲染</t>
   </si>
   <si>
     <t>音频播放</t>
   </si>
   <si>
-    <t>基于CoreAudio，音频播放的功能在AVTool中实现，需要添加进来，集成到工程中</t>
+    <t>windows基于CoreAudio，音频播放的功能在AVTool中实现，需要添加进来，集成到工程中</t>
+  </si>
+  <si>
+    <t>macOS基于AudioUnit，需要接入之前实现的逻辑</t>
   </si>
   <si>
     <t>视频帧缩略图</t>
@@ -1223,10 +1232,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9:J9"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1497,14 +1506,14 @@
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="10"/>
+      <c r="H17" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="I17" s="10"/>
       <c r="J17" s="10"/>
     </row>
     <row r="18" ht="39" customHeight="1" spans="1:10">
-      <c r="A18" s="6" t="s">
-        <v>30</v>
-      </c>
+      <c r="A18" s="6"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7" t="s">
         <v>31</v>
@@ -1513,9 +1522,11 @@
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
+      <c r="H18" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
     </row>
     <row r="19" ht="39" customHeight="1" spans="1:10">
       <c r="A19" s="6" t="s">
@@ -1533,29 +1544,27 @@
       <c r="I19" s="10"/>
       <c r="J19" s="10"/>
     </row>
-    <row r="20" ht="30" customHeight="1" spans="1:10">
-      <c r="A20" s="6" t="s">
-        <v>34</v>
-      </c>
+    <row r="20" ht="39" customHeight="1" spans="1:10">
+      <c r="A20" s="6"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-    </row>
-    <row r="21" ht="36" customHeight="1" spans="1:10">
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+    </row>
+    <row r="21" ht="39" customHeight="1" spans="1:10">
       <c r="A21" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
@@ -1565,13 +1574,13 @@
       <c r="I21" s="10"/>
       <c r="J21" s="10"/>
     </row>
-    <row r="22" ht="57" customHeight="1" spans="1:10">
+    <row r="22" ht="30" customHeight="1" spans="1:10">
       <c r="A22" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="6"/>
       <c r="C22" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
@@ -1581,10 +1590,14 @@
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
     </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="6"/>
+    <row r="23" ht="36" customHeight="1" spans="1:10">
+      <c r="A23" s="6" t="s">
+        <v>39</v>
+      </c>
       <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
+      <c r="C23" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -1593,10 +1606,14 @@
       <c r="I23" s="10"/>
       <c r="J23" s="10"/>
     </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="6"/>
+    <row r="24" ht="57" customHeight="1" spans="1:10">
+      <c r="A24" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
+      <c r="C24" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -1821,8 +1838,32 @@
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
     </row>
+    <row r="43" spans="1:10">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="10"/>
+      <c r="J43" s="10"/>
+    </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
+      <c r="J44" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="114">
+  <mergeCells count="118">
     <mergeCell ref="A5:J5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:G6"/>
@@ -1857,16 +1898,12 @@
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="C16:G16"/>
     <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B17"/>
     <mergeCell ref="C17:G17"/>
     <mergeCell ref="H17:J17"/>
-    <mergeCell ref="A18:B18"/>
     <mergeCell ref="C18:G18"/>
     <mergeCell ref="H18:J18"/>
-    <mergeCell ref="A19:B19"/>
     <mergeCell ref="C19:G19"/>
     <mergeCell ref="H19:J19"/>
-    <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A21:B21"/>
@@ -1935,8 +1972,16 @@
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="C42:G42"/>
     <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:G43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:G44"/>
+    <mergeCell ref="H44:J44"/>
     <mergeCell ref="A1:J2"/>
     <mergeCell ref="A3:J4"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
[improve] Add requirement points for customized UI
</commit_message>
<xml_diff>
--- a/documents/CSJVideoParser_dev_points.xlsx
+++ b/documents/CSJVideoParser_dev_points.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27555" windowHeight="11655"/>
+    <workbookView windowWidth="31830" windowHeight="12810"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>CSJVideoParser Version1.0.0</t>
   </si>
@@ -90,6 +90,17 @@
   <si>
     <t>1.去掉主界面上半部分当前选择/打开文件的UI，用大Logo和欢迎介绍语替换；
 2.主界面下半部分使用group UI，其中包含3个部分：播放器，多媒体数据分析，媒体格式工厂</t>
+  </si>
+  <si>
+    <t>开发主题管理模块</t>
+  </si>
+  <si>
+    <t>1.实现定制的CSJWidget，作为项目Widget的基类，拥有默认样式，支持自定义样式；
+2.主实现styleSheet文件管理，提供默认的styleSheets，以及新增定制styleSheets；</t>
+  </si>
+  <si>
+    <t>1.Customize windows to support round corner and shadow
+2.Customize render widget to support native rendering framework(Windowx-&gt;DirectX, MacoS-&gt;Metal)</t>
   </si>
   <si>
     <t>播放器功能实现</t>
@@ -922,7 +933,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -970,6 +981,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1349,10 +1366,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M47"/>
+  <dimension ref="A1:M48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:G7"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1487,7 +1504,7 @@
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
     </row>
-    <row r="8" ht="78" customHeight="1" spans="1:13">
+    <row r="8" ht="183" customHeight="1" spans="1:13">
       <c r="A8" s="14" t="s">
         <v>10</v>
       </c>
@@ -1500,21 +1517,23 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
       <c r="H8" s="9">
-        <v>46033</v>
+        <v>46046</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="11"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-    </row>
-    <row r="9" ht="87" customHeight="1" spans="1:13">
+      <c r="K8" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+    </row>
+    <row r="9" ht="78" customHeight="1" spans="1:13">
       <c r="A9" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
@@ -1529,662 +1548,683 @@
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
     </row>
-    <row r="10" ht="24" customHeight="1" spans="1:13">
+    <row r="10" ht="87" customHeight="1" spans="1:13">
       <c r="A10" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="15" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
+      <c r="H10" s="9">
+        <v>46033</v>
+      </c>
       <c r="I10" s="10"/>
       <c r="J10" s="11"/>
-      <c r="K10" s="12" t="s">
-        <v>16</v>
-      </c>
+      <c r="K10" s="12"/>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
     </row>
-    <row r="11" ht="37" customHeight="1" spans="1:13">
-      <c r="A11" s="17" t="s">
+    <row r="11" ht="24" customHeight="1" spans="1:13">
+      <c r="A11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="18"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
       <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="19" t="s">
+      <c r="I11" s="10"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="20"/>
-      <c r="M11" s="20"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
     </row>
     <row r="12" ht="37" customHeight="1" spans="1:13">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="19"/>
+      <c r="C12" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="19" t="s">
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="20"/>
-      <c r="M12" s="20"/>
-    </row>
-    <row r="13" ht="33" customHeight="1" spans="1:13">
-      <c r="A13" s="17" t="s">
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+    </row>
+    <row r="13" ht="37" customHeight="1" spans="1:13">
+      <c r="A13" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="17"/>
-      <c r="C13" s="18" t="s">
+      <c r="B13" s="19"/>
+      <c r="C13" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="21"/>
-    </row>
-    <row r="14" ht="24" customHeight="1" spans="1:13">
-      <c r="A14" s="17" t="s">
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="21" t="s">
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+    </row>
+    <row r="14" ht="33" customHeight="1" spans="1:13">
+      <c r="A14" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
-      <c r="K14" s="21"/>
-      <c r="L14" s="21"/>
-      <c r="M14" s="21"/>
-    </row>
-    <row r="15" ht="41" customHeight="1" spans="1:13">
-      <c r="A15" s="22" t="s">
+      <c r="B14" s="19"/>
+      <c r="C14" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="18" t="s">
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+    </row>
+    <row r="15" ht="24" customHeight="1" spans="1:13">
+      <c r="A15" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-    </row>
-    <row r="16" ht="25" customHeight="1" spans="1:13">
-      <c r="A16" s="17" t="s">
+      <c r="B15" s="19"/>
+      <c r="C15" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18" t="s">
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+    </row>
+    <row r="16" ht="41" customHeight="1" spans="1:13">
+      <c r="A16" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="19" t="s">
+      <c r="B16" s="24"/>
+      <c r="C16" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="L16" s="20"/>
-      <c r="M16" s="20"/>
-    </row>
-    <row r="17" ht="32" customHeight="1" spans="1:13">
-      <c r="A17" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18" t="s">
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+    </row>
+    <row r="17" ht="25" customHeight="1" spans="1:13">
+      <c r="A17" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-      <c r="K17" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="L17" s="20"/>
-      <c r="M17" s="20"/>
-    </row>
-    <row r="18" ht="46" customHeight="1" spans="1:13">
-      <c r="A18" s="17" t="s">
+      <c r="B17" s="19"/>
+      <c r="C17" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="18" t="s">
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+    </row>
+    <row r="18" ht="32" customHeight="1" spans="1:13">
+      <c r="A18" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21"/>
-      <c r="M18" s="21"/>
-    </row>
-    <row r="19" ht="41" customHeight="1" spans="1:13">
-      <c r="A19" s="17" t="s">
+      <c r="B18" s="19"/>
+      <c r="C18" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="18" t="s">
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22"/>
+    </row>
+    <row r="19" ht="46" customHeight="1" spans="1:13">
+      <c r="A19" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21"/>
-      <c r="M19" s="21"/>
-    </row>
-    <row r="20" ht="39" customHeight="1" spans="1:13">
-      <c r="A20" s="17" t="s">
+      <c r="B19" s="19"/>
+      <c r="C19" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="18" t="s">
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+    </row>
+    <row r="20" ht="41" customHeight="1" spans="1:13">
+      <c r="A20" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="21" t="s">
+      <c r="B20" s="19"/>
+      <c r="C20" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
     </row>
     <row r="21" ht="39" customHeight="1" spans="1:13">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18" t="s">
+      <c r="A21" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
-      <c r="F21" s="18"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="18"/>
-      <c r="I21" s="18"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="L21" s="18"/>
-      <c r="M21" s="18"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
     </row>
     <row r="22" ht="39" customHeight="1" spans="1:13">
-      <c r="A22" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18" t="s">
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="21"/>
-      <c r="L22" s="21"/>
-      <c r="M22" s="21"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="20"/>
     </row>
     <row r="23" ht="39" customHeight="1" spans="1:13">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
+      <c r="A23" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="19"/>
+      <c r="C23" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
     </row>
     <row r="24" ht="39" customHeight="1" spans="1:13">
-      <c r="A24" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="21"/>
-      <c r="L24" s="21"/>
-      <c r="M24" s="21"/>
-    </row>
-    <row r="25" ht="30" customHeight="1" spans="1:13">
-      <c r="A25" s="17" t="s">
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="18" t="s">
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="20"/>
+    </row>
+    <row r="25" ht="39" customHeight="1" spans="1:13">
+      <c r="A25" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
-    </row>
-    <row r="26" ht="36" customHeight="1" spans="1:13">
-      <c r="A26" s="17" t="s">
+      <c r="B25" s="19"/>
+      <c r="C25" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="18" t="s">
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+    </row>
+    <row r="26" ht="30" customHeight="1" spans="1:13">
+      <c r="A26" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="21"/>
-      <c r="M26" s="21"/>
-    </row>
-    <row r="27" ht="57" customHeight="1" spans="1:13">
-      <c r="A27" s="17" t="s">
+      <c r="B26" s="19"/>
+      <c r="C26" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18" t="s">
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+    </row>
+    <row r="27" ht="36" customHeight="1" spans="1:13">
+      <c r="A27" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="21"/>
-      <c r="M27" s="21"/>
-    </row>
-    <row r="28" spans="1:13">
-      <c r="A28" s="23"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
-      <c r="M28" s="25"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+    </row>
+    <row r="28" ht="57" customHeight="1" spans="1:13">
+      <c r="A28" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="19"/>
+      <c r="C28" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
     </row>
     <row r="29" spans="1:13">
-      <c r="A29" s="23"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="25"/>
-      <c r="M29" s="25"/>
+      <c r="A29" s="25"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="27"/>
     </row>
     <row r="30" spans="1:13">
-      <c r="A30" s="23"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="25"/>
-      <c r="L30" s="25"/>
-      <c r="M30" s="25"/>
+      <c r="A30" s="25"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="27"/>
+      <c r="M30" s="27"/>
     </row>
     <row r="31" spans="1:13">
-      <c r="A31" s="23"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="27"/>
+      <c r="M31" s="27"/>
     </row>
     <row r="32" spans="1:13">
-      <c r="A32" s="23"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="24"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="25"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+      <c r="K32" s="27"/>
+      <c r="L32" s="27"/>
+      <c r="M32" s="27"/>
     </row>
     <row r="33" spans="1:13">
-      <c r="A33" s="23"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
-      <c r="H33" s="24"/>
-      <c r="I33" s="24"/>
-      <c r="J33" s="24"/>
-      <c r="K33" s="25"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="25"/>
+      <c r="A33" s="25"/>
+      <c r="B33" s="25"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
+      <c r="K33" s="27"/>
+      <c r="L33" s="27"/>
+      <c r="M33" s="27"/>
     </row>
     <row r="34" spans="1:13">
-      <c r="A34" s="23"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="24"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
-      <c r="H34" s="24"/>
-      <c r="I34" s="24"/>
-      <c r="J34" s="24"/>
-      <c r="K34" s="25"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="25"/>
+      <c r="A34" s="25"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="26"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="26"/>
+      <c r="J34" s="26"/>
+      <c r="K34" s="27"/>
+      <c r="L34" s="27"/>
+      <c r="M34" s="27"/>
     </row>
     <row r="35" spans="1:13">
-      <c r="A35" s="23"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
-      <c r="H35" s="24"/>
-      <c r="I35" s="24"/>
-      <c r="J35" s="24"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="25"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="26"/>
+      <c r="H35" s="26"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="27"/>
+      <c r="L35" s="27"/>
+      <c r="M35" s="27"/>
     </row>
     <row r="36" spans="1:13">
-      <c r="A36" s="23"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
-      <c r="H36" s="24"/>
-      <c r="I36" s="24"/>
-      <c r="J36" s="24"/>
-      <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="25"/>
+      <c r="A36" s="25"/>
+      <c r="B36" s="25"/>
+      <c r="C36" s="26"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="26"/>
+      <c r="K36" s="27"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="27"/>
     </row>
     <row r="37" spans="1:13">
-      <c r="A37" s="23"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
-      <c r="H37" s="24"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="25"/>
-      <c r="L37" s="25"/>
-      <c r="M37" s="25"/>
+      <c r="A37" s="25"/>
+      <c r="B37" s="25"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="26"/>
+      <c r="G37" s="26"/>
+      <c r="H37" s="26"/>
+      <c r="I37" s="26"/>
+      <c r="J37" s="26"/>
+      <c r="K37" s="27"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="27"/>
     </row>
     <row r="38" spans="1:13">
-      <c r="A38" s="23"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="24"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
-      <c r="H38" s="24"/>
-      <c r="I38" s="24"/>
-      <c r="J38" s="24"/>
-      <c r="K38" s="25"/>
-      <c r="L38" s="25"/>
-      <c r="M38" s="25"/>
+      <c r="A38" s="25"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="26"/>
+      <c r="K38" s="27"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="27"/>
     </row>
     <row r="39" spans="1:13">
-      <c r="A39" s="23"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
-      <c r="J39" s="24"/>
-      <c r="K39" s="25"/>
-      <c r="L39" s="25"/>
-      <c r="M39" s="25"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="26"/>
+      <c r="F39" s="26"/>
+      <c r="G39" s="26"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="27"/>
+      <c r="L39" s="27"/>
+      <c r="M39" s="27"/>
     </row>
     <row r="40" spans="1:13">
-      <c r="A40" s="23"/>
-      <c r="B40" s="23"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="24"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="24"/>
-      <c r="K40" s="25"/>
-      <c r="L40" s="25"/>
-      <c r="M40" s="25"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="26"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="26"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="27"/>
     </row>
     <row r="41" spans="1:13">
-      <c r="A41" s="23"/>
-      <c r="B41" s="23"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="24"/>
-      <c r="F41" s="24"/>
-      <c r="G41" s="24"/>
-      <c r="H41" s="24"/>
-      <c r="I41" s="24"/>
-      <c r="J41" s="24"/>
-      <c r="K41" s="25"/>
-      <c r="L41" s="25"/>
-      <c r="M41" s="25"/>
+      <c r="A41" s="25"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="26"/>
+      <c r="G41" s="26"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="27"/>
+      <c r="L41" s="27"/>
+      <c r="M41" s="27"/>
     </row>
     <row r="42" spans="1:13">
-      <c r="A42" s="23"/>
-      <c r="B42" s="23"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="24"/>
-      <c r="F42" s="24"/>
-      <c r="G42" s="24"/>
-      <c r="H42" s="24"/>
-      <c r="I42" s="24"/>
-      <c r="J42" s="24"/>
-      <c r="K42" s="25"/>
-      <c r="L42" s="25"/>
-      <c r="M42" s="25"/>
+      <c r="A42" s="25"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="26"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="27"/>
+      <c r="L42" s="27"/>
+      <c r="M42" s="27"/>
     </row>
     <row r="43" spans="1:13">
-      <c r="A43" s="23"/>
-      <c r="B43" s="23"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="24"/>
-      <c r="G43" s="24"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="24"/>
-      <c r="J43" s="24"/>
-      <c r="K43" s="25"/>
-      <c r="L43" s="25"/>
-      <c r="M43" s="25"/>
+      <c r="A43" s="25"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="26"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="27"/>
+      <c r="M43" s="27"/>
     </row>
     <row r="44" spans="1:13">
-      <c r="A44" s="23"/>
-      <c r="B44" s="23"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24"/>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
-      <c r="H44" s="24"/>
-      <c r="I44" s="24"/>
-      <c r="J44" s="24"/>
-      <c r="K44" s="25"/>
-      <c r="L44" s="25"/>
-      <c r="M44" s="25"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="26"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
+      <c r="K44" s="27"/>
+      <c r="L44" s="27"/>
+      <c r="M44" s="27"/>
     </row>
     <row r="45" spans="1:13">
-      <c r="A45" s="23"/>
-      <c r="B45" s="23"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24"/>
-      <c r="K45" s="25"/>
-      <c r="L45" s="25"/>
-      <c r="M45" s="25"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="26"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
+      <c r="K45" s="27"/>
+      <c r="L45" s="27"/>
+      <c r="M45" s="27"/>
     </row>
     <row r="46" spans="1:13">
-      <c r="A46" s="23"/>
-      <c r="B46" s="23"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="24"/>
-      <c r="J46" s="24"/>
-      <c r="K46" s="25"/>
-      <c r="L46" s="25"/>
-      <c r="M46" s="25"/>
+      <c r="A46" s="25"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="27"/>
+      <c r="L46" s="27"/>
+      <c r="M46" s="27"/>
     </row>
     <row r="47" spans="1:13">
-      <c r="A47" s="23"/>
-      <c r="B47" s="23"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="24"/>
-      <c r="F47" s="24"/>
-      <c r="G47" s="24"/>
-      <c r="H47" s="24"/>
-      <c r="I47" s="24"/>
-      <c r="J47" s="24"/>
-      <c r="K47" s="25"/>
-      <c r="L47" s="25"/>
-      <c r="M47" s="25"/>
+      <c r="A47" s="25"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="26"/>
+      <c r="E47" s="26"/>
+      <c r="F47" s="26"/>
+      <c r="G47" s="26"/>
+      <c r="H47" s="26"/>
+      <c r="I47" s="26"/>
+      <c r="J47" s="26"/>
+      <c r="K47" s="27"/>
+      <c r="L47" s="27"/>
+      <c r="M47" s="27"/>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="25"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="26"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="26"/>
+      <c r="F48" s="26"/>
+      <c r="G48" s="26"/>
+      <c r="H48" s="26"/>
+      <c r="I48" s="26"/>
+      <c r="J48" s="26"/>
+      <c r="K48" s="27"/>
+      <c r="L48" s="27"/>
+      <c r="M48" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="127">
+  <mergeCells count="130">
     <mergeCell ref="A5:M5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="C6:G6"/>
@@ -2228,6 +2268,7 @@
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="C19:G19"/>
     <mergeCell ref="K19:M19"/>
+    <mergeCell ref="A20:B20"/>
     <mergeCell ref="C20:G20"/>
     <mergeCell ref="K20:M20"/>
     <mergeCell ref="C21:G21"/>
@@ -2236,7 +2277,6 @@
     <mergeCell ref="K22:M22"/>
     <mergeCell ref="C23:G23"/>
     <mergeCell ref="K23:M23"/>
-    <mergeCell ref="A24:B24"/>
     <mergeCell ref="C24:G24"/>
     <mergeCell ref="K24:M24"/>
     <mergeCell ref="A25:B25"/>
@@ -2308,10 +2348,13 @@
     <mergeCell ref="A47:B47"/>
     <mergeCell ref="C47:G47"/>
     <mergeCell ref="K47:M47"/>
-    <mergeCell ref="A20:B21"/>
-    <mergeCell ref="A22:B23"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="K48:M48"/>
     <mergeCell ref="A1:M2"/>
     <mergeCell ref="A3:M4"/>
+    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="A23:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>